<commit_message>
Add language option in Option
add language in option
</commit_message>
<xml_diff>
--- a/language/localization.xlsx
+++ b/language/localization.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27425"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Github Desktop Clone\Team-5\language\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6023357-B8E1-44AC-B055-249FEC13C1C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33FA0CDF-B027-4822-A736-DA231AADE215}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="16935" yWindow="5685" windowWidth="28800" windowHeight="15435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4845" yWindow="4650" windowWidth="28800" windowHeight="15345" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="20">
   <si>
     <t>en</t>
   </si>
@@ -33,12 +33,6 @@
     <t>zh</t>
   </si>
   <si>
-    <t>Start</t>
-  </si>
-  <si>
-    <t>开始</t>
-  </si>
-  <si>
     <t>Options</t>
   </si>
   <si>
@@ -67,6 +61,30 @@
   </si>
   <si>
     <t>主页</t>
+  </si>
+  <si>
+    <t>You Died</t>
+  </si>
+  <si>
+    <t>阵亡</t>
+  </si>
+  <si>
+    <t>Play Again</t>
+  </si>
+  <si>
+    <t>Return Home</t>
+  </si>
+  <si>
+    <t>返回主页</t>
+  </si>
+  <si>
+    <t>再次游玩</t>
+  </si>
+  <si>
+    <t>开始冒险</t>
+  </si>
+  <si>
+    <t>Start Adventure</t>
   </si>
 </sst>
 </file>
@@ -399,15 +417,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C7"/>
+  <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="19.5" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="18.42578125" customWidth="1"/>
+    <col min="1" max="1" width="18.42578125" style="1" customWidth="1"/>
     <col min="2" max="2" width="18.140625" style="1" customWidth="1"/>
     <col min="3" max="3" width="18.42578125" style="2" customWidth="1"/>
   </cols>
@@ -421,69 +439,102 @@
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A2" t="s">
+      <c r="A2" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C3" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C3" s="2" t="s">
+      <c r="B4" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A5" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A4" t="s">
-        <v>5</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C4" s="2" t="s">
+      <c r="B5" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A5" t="s">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A6" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="B6" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="C6" s="2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A6" t="s">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A7" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="B7" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C6" s="2" t="s">
+      <c r="C7" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A7" t="s">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A8" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="B8" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C7" s="2" t="s">
+      <c r="C8" s="2" t="s">
         <v>13</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A9" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A10" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add more translation language can change now
:(
</commit_message>
<xml_diff>
--- a/language/localization.xlsx
+++ b/language/localization.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Github Desktop Clone\Team-5\language\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33FA0CDF-B027-4822-A736-DA231AADE215}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69277765-EA15-4126-BB41-CF6EED63F5C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4845" yWindow="4650" windowWidth="28800" windowHeight="15345" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5640" yWindow="3285" windowWidth="28800" windowHeight="15345" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="34">
   <si>
     <t>en</t>
   </si>
@@ -85,6 +85,48 @@
   </si>
   <si>
     <t>Start Adventure</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Graphics: </t>
+  </si>
+  <si>
+    <t>图像</t>
+  </si>
+  <si>
+    <t>Volume:</t>
+  </si>
+  <si>
+    <t>Language:</t>
+  </si>
+  <si>
+    <t>语言</t>
+  </si>
+  <si>
+    <t>Settings</t>
+  </si>
+  <si>
+    <t>设置</t>
+  </si>
+  <si>
+    <t>Deep Dive Descent</t>
+  </si>
+  <si>
+    <t>深浅迷航</t>
+  </si>
+  <si>
+    <t>Language</t>
+  </si>
+  <si>
+    <t>Return</t>
+  </si>
+  <si>
+    <t>English</t>
+  </si>
+  <si>
+    <t>Chinese</t>
+  </si>
+  <si>
+    <t>中文</t>
   </si>
 </sst>
 </file>
@@ -417,10 +459,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C10"/>
+  <dimension ref="A1:C19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="19.5" x14ac:dyDescent="0.45"/>
@@ -537,6 +579,105 @@
         <v>16</v>
       </c>
     </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A11" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A12" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A13" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A14" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A15" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A16" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A17" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A18" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A19" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
updated ui, pause menu, added transitions, added music
</commit_message>
<xml_diff>
--- a/language/localization.xlsx
+++ b/language/localization.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27425"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Github Desktop Clone\Team-5\language\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6023357-B8E1-44AC-B055-249FEC13C1C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69277765-EA15-4126-BB41-CF6EED63F5C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="16935" yWindow="5685" windowWidth="28800" windowHeight="15435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5640" yWindow="3285" windowWidth="28800" windowHeight="15345" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="34">
   <si>
     <t>en</t>
   </si>
@@ -33,12 +33,6 @@
     <t>zh</t>
   </si>
   <si>
-    <t>Start</t>
-  </si>
-  <si>
-    <t>开始</t>
-  </si>
-  <si>
     <t>Options</t>
   </si>
   <si>
@@ -67,6 +61,72 @@
   </si>
   <si>
     <t>主页</t>
+  </si>
+  <si>
+    <t>You Died</t>
+  </si>
+  <si>
+    <t>阵亡</t>
+  </si>
+  <si>
+    <t>Play Again</t>
+  </si>
+  <si>
+    <t>Return Home</t>
+  </si>
+  <si>
+    <t>返回主页</t>
+  </si>
+  <si>
+    <t>再次游玩</t>
+  </si>
+  <si>
+    <t>开始冒险</t>
+  </si>
+  <si>
+    <t>Start Adventure</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Graphics: </t>
+  </si>
+  <si>
+    <t>图像</t>
+  </si>
+  <si>
+    <t>Volume:</t>
+  </si>
+  <si>
+    <t>Language:</t>
+  </si>
+  <si>
+    <t>语言</t>
+  </si>
+  <si>
+    <t>Settings</t>
+  </si>
+  <si>
+    <t>设置</t>
+  </si>
+  <si>
+    <t>Deep Dive Descent</t>
+  </si>
+  <si>
+    <t>深浅迷航</t>
+  </si>
+  <si>
+    <t>Language</t>
+  </si>
+  <si>
+    <t>Return</t>
+  </si>
+  <si>
+    <t>English</t>
+  </si>
+  <si>
+    <t>Chinese</t>
+  </si>
+  <si>
+    <t>中文</t>
   </si>
 </sst>
 </file>
@@ -399,15 +459,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C7"/>
+  <dimension ref="A1:C19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="19.5" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="18.42578125" customWidth="1"/>
+    <col min="1" max="1" width="18.42578125" style="1" customWidth="1"/>
     <col min="2" max="2" width="18.140625" style="1" customWidth="1"/>
     <col min="3" max="3" width="18.42578125" style="2" customWidth="1"/>
   </cols>
@@ -421,69 +481,201 @@
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A2" t="s">
+      <c r="A2" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C3" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C3" s="2" t="s">
+      <c r="B4" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A5" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A4" t="s">
-        <v>5</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C4" s="2" t="s">
+      <c r="B5" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A5" t="s">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A6" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="B6" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="C6" s="2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A6" t="s">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A7" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="B7" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C6" s="2" t="s">
+      <c r="C7" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A7" t="s">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A8" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="B8" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C7" s="2" t="s">
+      <c r="C8" s="2" t="s">
         <v>13</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A9" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A10" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A11" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A12" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A13" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A14" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A15" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A16" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A17" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A18" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A19" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>33</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fix some code add more translate
</commit_message>
<xml_diff>
--- a/language/localization.xlsx
+++ b/language/localization.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Github Desktop Clone\Team-5\language\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69277765-EA15-4126-BB41-CF6EED63F5C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62B6D1CD-757E-4F97-86F7-7C0899D6EC9B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5640" yWindow="3285" windowWidth="28800" windowHeight="15345" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4950" yWindow="4680" windowWidth="28800" windowHeight="15345" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="69">
   <si>
     <t>en</t>
   </si>
@@ -127,6 +127,111 @@
   </si>
   <si>
     <t>中文</t>
+  </si>
+  <si>
+    <t>音频</t>
+  </si>
+  <si>
+    <t>操作</t>
+  </si>
+  <si>
+    <t>全屏</t>
+  </si>
+  <si>
+    <t>无边框</t>
+  </si>
+  <si>
+    <t>Fullscreen</t>
+  </si>
+  <si>
+    <t>Video</t>
+  </si>
+  <si>
+    <t>Audio</t>
+  </si>
+  <si>
+    <t>Controls</t>
+  </si>
+  <si>
+    <t>Borderless</t>
+  </si>
+  <si>
+    <t>Disabled</t>
+  </si>
+  <si>
+    <t>Enabled</t>
+  </si>
+  <si>
+    <t>Adaptive</t>
+  </si>
+  <si>
+    <t>Nvidia DLSS</t>
+  </si>
+  <si>
+    <t>自适应</t>
+  </si>
+  <si>
+    <t>关闭</t>
+  </si>
+  <si>
+    <t>开启</t>
+  </si>
+  <si>
+    <t>Master</t>
+  </si>
+  <si>
+    <t>Master_Music</t>
+  </si>
+  <si>
+    <t>主音量</t>
+  </si>
+  <si>
+    <t>Music</t>
+  </si>
+  <si>
+    <t>音乐</t>
+  </si>
+  <si>
+    <t>SFX</t>
+  </si>
+  <si>
+    <t>音效</t>
+  </si>
+  <si>
+    <t>Game</t>
+  </si>
+  <si>
+    <t>游戏</t>
+  </si>
+  <si>
+    <t>Paused_Settings</t>
+  </si>
+  <si>
+    <t>settings</t>
+  </si>
+  <si>
+    <t>Resume</t>
+  </si>
+  <si>
+    <t>恢复游戏</t>
+  </si>
+  <si>
+    <t>Restart</t>
+  </si>
+  <si>
+    <t>重新开始</t>
+  </si>
+  <si>
+    <t>Main Menu</t>
+  </si>
+  <si>
+    <t>主菜单</t>
+  </si>
+  <si>
+    <t>Game Paused</t>
+  </si>
+  <si>
+    <t>游戏暂停</t>
   </si>
 </sst>
 </file>
@@ -459,10 +564,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C19"/>
+  <dimension ref="A1:C38"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="C38" sqref="C38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="19.5" x14ac:dyDescent="0.45"/>
@@ -678,6 +783,215 @@
         <v>33</v>
       </c>
     </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A20" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A21" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A22" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A23" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A24" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A25" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A26" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A27" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A28" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A29" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="C29" s="2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A30" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="C30" s="2" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A31" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="C31" s="2" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A32" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="C32" s="2" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A33" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="C33" s="2" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A34" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="C34" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A35" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="C35" s="2" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A36" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="C36" s="2" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A37" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="C37" s="2" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A38" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="C38" s="2" t="s">
+        <v>68</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Idle Animation follows cursor, Cleaned up player code
</commit_message>
<xml_diff>
--- a/language/localization.xlsx
+++ b/language/localization.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27425"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Github Desktop Clone\Team-5\language\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6023357-B8E1-44AC-B055-249FEC13C1C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69277765-EA15-4126-BB41-CF6EED63F5C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="16935" yWindow="5685" windowWidth="28800" windowHeight="15435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5640" yWindow="3285" windowWidth="28800" windowHeight="15345" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="34">
   <si>
     <t>en</t>
   </si>
@@ -33,12 +33,6 @@
     <t>zh</t>
   </si>
   <si>
-    <t>Start</t>
-  </si>
-  <si>
-    <t>开始</t>
-  </si>
-  <si>
     <t>Options</t>
   </si>
   <si>
@@ -67,6 +61,72 @@
   </si>
   <si>
     <t>主页</t>
+  </si>
+  <si>
+    <t>You Died</t>
+  </si>
+  <si>
+    <t>阵亡</t>
+  </si>
+  <si>
+    <t>Play Again</t>
+  </si>
+  <si>
+    <t>Return Home</t>
+  </si>
+  <si>
+    <t>返回主页</t>
+  </si>
+  <si>
+    <t>再次游玩</t>
+  </si>
+  <si>
+    <t>开始冒险</t>
+  </si>
+  <si>
+    <t>Start Adventure</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Graphics: </t>
+  </si>
+  <si>
+    <t>图像</t>
+  </si>
+  <si>
+    <t>Volume:</t>
+  </si>
+  <si>
+    <t>Language:</t>
+  </si>
+  <si>
+    <t>语言</t>
+  </si>
+  <si>
+    <t>Settings</t>
+  </si>
+  <si>
+    <t>设置</t>
+  </si>
+  <si>
+    <t>Deep Dive Descent</t>
+  </si>
+  <si>
+    <t>深浅迷航</t>
+  </si>
+  <si>
+    <t>Language</t>
+  </si>
+  <si>
+    <t>Return</t>
+  </si>
+  <si>
+    <t>English</t>
+  </si>
+  <si>
+    <t>Chinese</t>
+  </si>
+  <si>
+    <t>中文</t>
   </si>
 </sst>
 </file>
@@ -399,15 +459,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C7"/>
+  <dimension ref="A1:C19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="19.5" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="18.42578125" customWidth="1"/>
+    <col min="1" max="1" width="18.42578125" style="1" customWidth="1"/>
     <col min="2" max="2" width="18.140625" style="1" customWidth="1"/>
     <col min="3" max="3" width="18.42578125" style="2" customWidth="1"/>
   </cols>
@@ -421,69 +481,201 @@
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A2" t="s">
+      <c r="A2" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C3" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C3" s="2" t="s">
+      <c r="B4" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A5" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A4" t="s">
-        <v>5</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C4" s="2" t="s">
+      <c r="B5" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A5" t="s">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A6" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="B6" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="C6" s="2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A6" t="s">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A7" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="B7" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C6" s="2" t="s">
+      <c r="C7" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A7" t="s">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A8" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="B8" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C7" s="2" t="s">
+      <c r="C8" s="2" t="s">
         <v>13</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A9" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A10" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A11" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A12" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A13" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A14" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A15" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A16" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A17" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A18" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A19" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>33</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added more idle animations, cleaned up code
</commit_message>
<xml_diff>
--- a/language/localization.xlsx
+++ b/language/localization.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Github Desktop Clone\Team-5\language\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69277765-EA15-4126-BB41-CF6EED63F5C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62B6D1CD-757E-4F97-86F7-7C0899D6EC9B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5640" yWindow="3285" windowWidth="28800" windowHeight="15345" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4950" yWindow="4680" windowWidth="28800" windowHeight="15345" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="69">
   <si>
     <t>en</t>
   </si>
@@ -127,6 +127,111 @@
   </si>
   <si>
     <t>中文</t>
+  </si>
+  <si>
+    <t>音频</t>
+  </si>
+  <si>
+    <t>操作</t>
+  </si>
+  <si>
+    <t>全屏</t>
+  </si>
+  <si>
+    <t>无边框</t>
+  </si>
+  <si>
+    <t>Fullscreen</t>
+  </si>
+  <si>
+    <t>Video</t>
+  </si>
+  <si>
+    <t>Audio</t>
+  </si>
+  <si>
+    <t>Controls</t>
+  </si>
+  <si>
+    <t>Borderless</t>
+  </si>
+  <si>
+    <t>Disabled</t>
+  </si>
+  <si>
+    <t>Enabled</t>
+  </si>
+  <si>
+    <t>Adaptive</t>
+  </si>
+  <si>
+    <t>Nvidia DLSS</t>
+  </si>
+  <si>
+    <t>自适应</t>
+  </si>
+  <si>
+    <t>关闭</t>
+  </si>
+  <si>
+    <t>开启</t>
+  </si>
+  <si>
+    <t>Master</t>
+  </si>
+  <si>
+    <t>Master_Music</t>
+  </si>
+  <si>
+    <t>主音量</t>
+  </si>
+  <si>
+    <t>Music</t>
+  </si>
+  <si>
+    <t>音乐</t>
+  </si>
+  <si>
+    <t>SFX</t>
+  </si>
+  <si>
+    <t>音效</t>
+  </si>
+  <si>
+    <t>Game</t>
+  </si>
+  <si>
+    <t>游戏</t>
+  </si>
+  <si>
+    <t>Paused_Settings</t>
+  </si>
+  <si>
+    <t>settings</t>
+  </si>
+  <si>
+    <t>Resume</t>
+  </si>
+  <si>
+    <t>恢复游戏</t>
+  </si>
+  <si>
+    <t>Restart</t>
+  </si>
+  <si>
+    <t>重新开始</t>
+  </si>
+  <si>
+    <t>Main Menu</t>
+  </si>
+  <si>
+    <t>主菜单</t>
+  </si>
+  <si>
+    <t>Game Paused</t>
+  </si>
+  <si>
+    <t>游戏暂停</t>
   </si>
 </sst>
 </file>
@@ -459,10 +564,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C19"/>
+  <dimension ref="A1:C38"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="C38" sqref="C38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="19.5" x14ac:dyDescent="0.45"/>
@@ -678,6 +783,215 @@
         <v>33</v>
       </c>
     </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A20" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A21" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A22" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A23" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A24" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A25" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A26" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A27" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A28" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A29" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="C29" s="2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A30" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="C30" s="2" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A31" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="C31" s="2" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A32" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="C32" s="2" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A33" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="C33" s="2" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A34" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="C34" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A35" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="C35" s="2" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A36" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="C36" s="2" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A37" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="C37" s="2" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A38" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="C38" s="2" t="s">
+        <v>68</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>